<commit_message>
Ajout des erratas datasheets pic
</commit_message>
<xml_diff>
--- a/Schémas Electriques/Schémas V2 - wrapping/Schémas V2 - BOM.xlsx
+++ b/Schémas Electriques/Schémas V2 - wrapping/Schémas V2 - BOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="405" windowWidth="28275" windowHeight="13080"/>
@@ -11,12 +11,12 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="96">
   <si>
     <t>Report Generated From Altium Designer</t>
   </si>
@@ -111,9 +111,6 @@
     <t>D3</t>
   </si>
   <si>
-    <t>Schottky Diode</t>
-  </si>
-  <si>
     <t>J1, J2</t>
   </si>
   <si>
@@ -153,9 +150,6 @@
     <t>Q2</t>
   </si>
   <si>
-    <t>NPN Bipolar Transistor</t>
-  </si>
-  <si>
     <t>R1, R3, R5, R11, R18, R22</t>
   </si>
   <si>
@@ -280,13 +274,43 @@
   </si>
   <si>
     <t>C9, C13, Cap1, Cap2, Cap3, Cap4</t>
+  </si>
+  <si>
+    <t>Référence</t>
+  </si>
+  <si>
+    <t>RS : 535-9256</t>
+  </si>
+  <si>
+    <t>RS : 535-9262</t>
+  </si>
+  <si>
+    <t>NPN Bipolar Transistor BC237</t>
+  </si>
+  <si>
+    <t>RS : 625-4691</t>
+  </si>
+  <si>
+    <t>Farn : 952-4851</t>
+  </si>
+  <si>
+    <t>RS : 540-8538</t>
+  </si>
+  <si>
+    <t>Schottky Diode 1N5820</t>
+  </si>
+  <si>
+    <t>774-3341</t>
+  </si>
+  <si>
+    <t>Farn : 9493719</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -486,7 +510,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -521,7 +544,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -697,21 +719,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="45.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="11"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -719,7 +742,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="8"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
@@ -732,8 +755,11 @@
       <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -747,7 +773,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -761,7 +787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -775,7 +801,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -789,7 +815,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
@@ -803,7 +829,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
@@ -817,7 +843,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
@@ -831,7 +857,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -845,9 +871,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>6</v>
@@ -859,7 +885,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
@@ -873,251 +899,263 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="D22" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="3" t="s">
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="B23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="D23" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="B24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="B27" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="3" t="s">
+      <c r="B29" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="D29" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="3" t="s">
+      <c r="B30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D29" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="D30" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C30" s="3" t="s">
+      <c r="B31" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>13</v>
@@ -1130,15 +1168,15 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>13</v>
@@ -1151,12 +1189,12 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="10" t="s">
@@ -1170,12 +1208,12 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="A34" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="10" t="s">
@@ -1189,12 +1227,12 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="A35" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="10" t="s">
@@ -1208,18 +1246,20 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E36" s="1"/>
+      <c r="E36" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -1227,18 +1267,20 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="A37" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="1"/>
+      <c r="E37" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -1246,18 +1288,20 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11">
       <c r="A38" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E38" s="1"/>
+      <c r="E38" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
@@ -1265,12 +1309,12 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11">
       <c r="A39" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="10" t="s">
@@ -1284,9 +1328,9 @@
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11">
       <c r="A40" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1298,7 +1342,7 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1308,24 +1352,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>